<commit_message>
Updated Excel files. Small tweaks to other code nothing major.
</commit_message>
<xml_diff>
--- a/Clustering/May_17_Clustering_Results.xlsx
+++ b/Clustering/May_17_Clustering_Results.xlsx
@@ -31,214 +31,214 @@
     <t>Facility Affiliations</t>
   </si>
   <si>
-    <t>[1, 53, 283, 54, 55]</t>
-  </si>
-  <si>
-    <t>[285, 289, 0, 53, 283, 7, 35, 6]</t>
-  </si>
-  <si>
-    <t>[108, 127, 69, 184, 175, 109, 177, 176]</t>
-  </si>
-  <si>
-    <t>[56, 54, 57, 264, 211, 268, 266, 267]</t>
-  </si>
-  <si>
-    <t>[290, 7, 6, 180, 179, 178]</t>
-  </si>
-  <si>
-    <t>[82, 465, 166, 174, 175, 172, 141, 154, 153]</t>
-  </si>
-  <si>
-    <t>[1, 7, 35, 174, 179, 172, 173, 4]</t>
-  </si>
-  <si>
-    <t>[388, 289, 1, 292, 291, 290, 6, 4]</t>
-  </si>
-  <si>
-    <t>[153, 11, 76, 139, 136, 135, 14]</t>
-  </si>
-  <si>
-    <t>[156, 65, 24, 77, 26]</t>
-  </si>
-  <si>
-    <t>[200, 198, 199, 18, 26, 133, 140]</t>
-  </si>
-  <si>
-    <t>[156, 155, 153, 77, 8, 19, 139]</t>
-  </si>
-  <si>
-    <t>[16, 15, 17, 131, 133]</t>
+    <t>[283, 1, 53, 55, 54]</t>
+  </si>
+  <si>
+    <t>[289, 7, 285, 283, 6, 35, 53, 0]</t>
+  </si>
+  <si>
+    <t>[127, 184, 175, 177, 69, 108, 176, 109]</t>
+  </si>
+  <si>
+    <t>[264, 266, 268, 211, 267, 56, 57, 54]</t>
+  </si>
+  <si>
+    <t>[290, 7, 6, 178, 179, 180]</t>
+  </si>
+  <si>
+    <t>[82, 141, 175, 172, 166, 465, 174, 153, 154]</t>
+  </si>
+  <si>
+    <t>[7, 4, 179, 172, 1, 174, 35, 173]</t>
+  </si>
+  <si>
+    <t>[289, 388, 291, 290, 1, 292, 6, 4]</t>
+  </si>
+  <si>
+    <t>[76, 135, 153, 136, 11, 139, 14]</t>
+  </si>
+  <si>
+    <t>[65, 24, 156, 26, 77]</t>
+  </si>
+  <si>
+    <t>[140, 18, 133, 199, 200, 198, 26]</t>
+  </si>
+  <si>
+    <t>[155, 153, 8, 156, 19, 139, 77]</t>
+  </si>
+  <si>
+    <t>[15, 16, 17, 131, 133]</t>
   </si>
   <si>
     <t>[35, 52, 173]</t>
   </si>
   <si>
-    <t>[15, 133, 136, 8, 76, 267, 199]</t>
-  </si>
-  <si>
-    <t>[136, 137, 16, 135, 12, 133, 14]</t>
-  </si>
-  <si>
-    <t>[139, 19, 137, 131, 12, 15]</t>
+    <t>[136, 15, 133, 199, 267, 76, 8]</t>
+  </si>
+  <si>
+    <t>[135, 137, 136, 133, 12, 16, 14]</t>
+  </si>
+  <si>
+    <t>[137, 15, 19, 139, 12, 131]</t>
   </si>
   <si>
     <t>[131, 12, 138, 133]</t>
   </si>
   <si>
-    <t>[133, 10, 138, 140]</t>
-  </si>
-  <si>
-    <t>[11, 139, 77, 131, 16]</t>
-  </si>
-  <si>
-    <t>[23, 198, 21, 26]</t>
-  </si>
-  <si>
-    <t>[25, 22, 23, 24, 20, 200, 198]</t>
-  </si>
-  <si>
-    <t>[196, 25, 202, 216, 21, 200]</t>
-  </si>
-  <si>
-    <t>[26, 24, 20, 21]</t>
-  </si>
-  <si>
-    <t>[66, 65, 25, 9, 23, 21, 26]</t>
-  </si>
-  <si>
-    <t>[66, 195, 196, 24, 22, 21]</t>
-  </si>
-  <si>
-    <t>[9, 23, 24, 20, 198, 77, 10, 140]</t>
-  </si>
-  <si>
-    <t>[28, 150, 194, 149, 64]</t>
-  </si>
-  <si>
-    <t>[61, 60, 247, 63, 27, 194, 150, 197]</t>
-  </si>
-  <si>
-    <t>[64, 146, 118, 151, 63, 49]</t>
-  </si>
-  <si>
-    <t>[31, 51, 34, 32, 49, 205]</t>
-  </si>
-  <si>
-    <t>[33, 30, 51, 32]</t>
-  </si>
-  <si>
-    <t>[33, 31, 34, 30, 81]</t>
-  </si>
-  <si>
-    <t>[31, 32, 206, 50, 51, 204, 81]</t>
-  </si>
-  <si>
-    <t>[81, 32, 467, 30, 205]</t>
-  </si>
-  <si>
-    <t>[53, 1, 13, 52, 6, 173]</t>
-  </si>
-  <si>
-    <t>[256, 282, 257, 248, 230, 231, 229]</t>
-  </si>
-  <si>
-    <t>[265, 42, 38, 40, 211]</t>
-  </si>
-  <si>
-    <t>[42, 37, 211, 39]</t>
-  </si>
-  <si>
-    <t>[42, 38, 216, 211, 41]</t>
-  </si>
-  <si>
-    <t>[265, 42, 41, 37]</t>
-  </si>
-  <si>
-    <t>[213, 158, 265, 42, 39, 216, 40]</t>
-  </si>
-  <si>
-    <t>[38, 39, 41, 40, 37]</t>
-  </si>
-  <si>
-    <t>[44, 204, 126, 110, 122]</t>
-  </si>
-  <si>
-    <t>[43, 204, 122, 84, 45, 91, 106]</t>
+    <t>[74, 140, 133, 138, 10]</t>
+  </si>
+  <si>
+    <t>[139, 11, 77, 131, 16]</t>
+  </si>
+  <si>
+    <t>[23, 21, 198, 26]</t>
+  </si>
+  <si>
+    <t>[25, 22, 23, 24, 200, 198, 20]</t>
+  </si>
+  <si>
+    <t>[216, 202, 196, 25, 200, 21]</t>
+  </si>
+  <si>
+    <t>[21, 24, 20, 26]</t>
+  </si>
+  <si>
+    <t>[65, 66, 25, 23, 21, 9, 26]</t>
+  </si>
+  <si>
+    <t>[195, 66, 196, 24, 22, 21]</t>
+  </si>
+  <si>
+    <t>[23, 24, 20, 198, 9, 74, 77, 140, 10]</t>
+  </si>
+  <si>
+    <t>[194, 28, 150, 149, 64]</t>
+  </si>
+  <si>
+    <t>[60, 61, 27, 247, 63, 194, 150, 197]</t>
+  </si>
+  <si>
+    <t>[63, 49, 64, 146, 151, 118]</t>
+  </si>
+  <si>
+    <t>[49, 31, 51, 34, 205, 32]</t>
+  </si>
+  <si>
+    <t>[33, 32, 30, 51]</t>
+  </si>
+  <si>
+    <t>[31, 33, 34, 30, 81]</t>
+  </si>
+  <si>
+    <t>[50, 206, 204, 31, 51, 81, 32]</t>
+  </si>
+  <si>
+    <t>[30, 32, 205, 81, 79]</t>
+  </si>
+  <si>
+    <t>[1, 6, 53, 13, 52, 173]</t>
+  </si>
+  <si>
+    <t>[282, 256, 257, 248, 230, 231, 229]</t>
+  </si>
+  <si>
+    <t>[40, 265, 38, 42, 211]</t>
+  </si>
+  <si>
+    <t>[42, 39, 37, 211]</t>
+  </si>
+  <si>
+    <t>[216, 41, 38, 42, 211]</t>
+  </si>
+  <si>
+    <t>[42, 41, 37, 265]</t>
+  </si>
+  <si>
+    <t>[158, 213, 216, 40, 39, 42, 265]</t>
+  </si>
+  <si>
+    <t>[40, 41, 38, 39, 37]</t>
+  </si>
+  <si>
+    <t>[204, 126, 122, 110, 44]</t>
+  </si>
+  <si>
+    <t>[204, 84, 45, 106, 122, 43, 91]</t>
   </si>
   <si>
     <t>[188, 204, 84, 44, 85]</t>
   </si>
   <si>
-    <t>[92, 62, 59, 51, 103, 48, 50]</t>
-  </si>
-  <si>
-    <t>[97, 99, 98, 106, 83, 85, 104, 129, 105]</t>
-  </si>
-  <si>
-    <t>[46, 103, 50, 206]</t>
-  </si>
-  <si>
-    <t>[59, 51, 30, 29, 63, 118, 205, 120]</t>
-  </si>
-  <si>
-    <t>[46, 48, 33, 206, 51]</t>
-  </si>
-  <si>
-    <t>[59, 46, 33, 31, 50, 49, 30]</t>
-  </si>
-  <si>
-    <t>[53, 54, 13, 35, 267, 173]</t>
-  </si>
-  <si>
-    <t>[0, 52, 54, 35, 1]</t>
-  </si>
-  <si>
-    <t>[56, 3, 0, 53, 55, 52, 267]</t>
-  </si>
-  <si>
-    <t>[56, 57, 0, 283, 54]</t>
-  </si>
-  <si>
-    <t>[54, 55, 57, 3]</t>
-  </si>
-  <si>
-    <t>[380, 56, 3, 285, 284, 55, 266, 283]</t>
-  </si>
-  <si>
-    <t>[147, 150, 148, 149, 64]</t>
-  </si>
-  <si>
-    <t>[62, 49, 51, 46, 60, 63]</t>
-  </si>
-  <si>
-    <t>[62, 61, 59, 28, 63]</t>
-  </si>
-  <si>
-    <t>[62, 228, 60, 28, 220, 227, 466, 236, 247]</t>
-  </si>
-  <si>
-    <t>[237, 92, 46, 59, 228, 61, 60]</t>
-  </si>
-  <si>
-    <t>[59, 60, 152, 28, 150, 29, 151, 49]</t>
-  </si>
-  <si>
-    <t>[68, 194, 148, 27, 149, 58, 66, 29, 146, 67, 118, 119]</t>
-  </si>
-  <si>
-    <t>[66, 67, 156, 155, 24, 154, 9]</t>
-  </si>
-  <si>
-    <t>[68, 195, 24, 65, 64, 25, 67]</t>
-  </si>
-  <si>
-    <t>[66, 64, 65, 154, 119]</t>
-  </si>
-  <si>
-    <t>[191, 190, 193, 192, 195, 189, 194, 66, 64]</t>
-  </si>
-  <si>
-    <t>[127, 292, 291, 2, 175, 290, 178, 181]</t>
+    <t>[92, 59, 62, 103, 51, 48, 50]</t>
+  </si>
+  <si>
+    <t>[97, 99, 98, 83, 85, 106, 104, 129, 105]</t>
+  </si>
+  <si>
+    <t>[103, 46, 206, 50]</t>
+  </si>
+  <si>
+    <t>[59, 29, 118, 63, 51, 120, 205, 30]</t>
+  </si>
+  <si>
+    <t>[46, 48, 51, 206, 33]</t>
+  </si>
+  <si>
+    <t>[59, 46, 50, 49, 31, 33, 30]</t>
+  </si>
+  <si>
+    <t>[53, 13, 35, 173, 267, 54]</t>
+  </si>
+  <si>
+    <t>[1, 35, 52, 0, 54]</t>
+  </si>
+  <si>
+    <t>[53, 0, 52, 267, 56, 3, 55]</t>
+  </si>
+  <si>
+    <t>[283, 0, 56, 57, 54]</t>
+  </si>
+  <si>
+    <t>[3, 57, 54, 55]</t>
+  </si>
+  <si>
+    <t>[285, 284, 380, 283, 266, 56, 3, 55]</t>
+  </si>
+  <si>
+    <t>[149, 147, 150, 64, 148]</t>
+  </si>
+  <si>
+    <t>[60, 49, 51, 46, 62, 63]</t>
+  </si>
+  <si>
+    <t>[59, 62, 61, 63, 28]</t>
+  </si>
+  <si>
+    <t>[60, 62, 228, 28, 220, 227, 466, 236, 247]</t>
+  </si>
+  <si>
+    <t>[237, 92, 60, 59, 46, 228, 61]</t>
+  </si>
+  <si>
+    <t>[60, 59, 29, 28, 152, 49, 150, 151]</t>
+  </si>
+  <si>
+    <t>[27, 149, 29, 119, 118, 58, 146, 148, 194, 66, 67, 68]</t>
+  </si>
+  <si>
+    <t>[67, 154, 66, 155, 156, 9, 24]</t>
+  </si>
+  <si>
+    <t>[64, 67, 68, 65, 195, 24, 25]</t>
+  </si>
+  <si>
+    <t>[119, 64, 66, 154, 65]</t>
+  </si>
+  <si>
+    <t>[64, 194, 192, 193, 191, 189, 190, 66, 195]</t>
+  </si>
+  <si>
+    <t>[291, 127, 2, 290, 292, 181, 175, 178]</t>
   </si>
   <si>
     <t>[168, 95, 170, 464, 96]</t>
@@ -250,28 +250,28 @@
     <t>[93, 80, 129, 130, 128]</t>
   </si>
   <si>
-    <t>[173, 153, 267, 8, 135, 14]</t>
-  </si>
-  <si>
-    <t>[156, 11, 9, 19, 26, 132, 131, 140]</t>
-  </si>
-  <si>
-    <t>[184, 166, 205, 467, 125, 177, 79]</t>
-  </si>
-  <si>
-    <t>[81, 467, 125, 78, 124]</t>
-  </si>
-  <si>
-    <t>[71, 96, 93, 72, 464, 405, 356, 128, 127]</t>
-  </si>
-  <si>
-    <t>[33, 204, 34, 32, 126, 124, 467, 79]</t>
+    <t>[8, 153, 173, 267, 135, 14]</t>
+  </si>
+  <si>
+    <t>[9, 156, 19, 11, 26, 131, 140, 132]</t>
+  </si>
+  <si>
+    <t>[125, 79, 177, 184, 166, 205]</t>
+  </si>
+  <si>
+    <t>[124, 34, 81, 78, 125, 205]</t>
+  </si>
+  <si>
+    <t>[71, 96, 93, 464, 405, 356, 72, 127, 128]</t>
+  </si>
+  <si>
+    <t>[124, 204, 126, 33, 34, 32, 79]</t>
   </si>
   <si>
     <t>[184, 175, 166, 5]</t>
   </si>
   <si>
-    <t>[84, 106, 47, 85]</t>
+    <t>[84, 47, 106, 85]</t>
   </si>
   <si>
     <t>[44, 106, 83, 45, 85]</t>
@@ -280,7 +280,7 @@
     <t>[188, 99, 84, 83, 45, 47]</t>
   </si>
   <si>
-    <t>[87, 91, 90, 106]</t>
+    <t>[87, 90, 106, 91]</t>
   </si>
   <si>
     <t>[106, 86, 88, 90]</t>
@@ -292,10 +292,10 @@
     <t>[88, 130, 104, 105, 129]</t>
   </si>
   <si>
-    <t>[87, 86, 88, 130, 108, 91, 128]</t>
-  </si>
-  <si>
-    <t>[86, 122, 44, 106, 108, 121, 90]</t>
+    <t>[128, 87, 88, 130, 108, 86, 91]</t>
+  </si>
+  <si>
+    <t>[90, 86, 106, 108, 122, 121, 44]</t>
   </si>
   <si>
     <t>[167, 102, 237, 62, 182, 46, 103]</t>
@@ -304,7 +304,7 @@
     <t>[95, 71, 80, 72, 114, 117, 101, 129]</t>
   </si>
   <si>
-    <t>[269, 245, 278, 212]</t>
+    <t>[269, 278, 245, 212]</t>
   </si>
   <si>
     <t>[93, 117, 71, 170, 70, 96, 169]</t>
@@ -331,7 +331,7 @@
     <t>[171, 167, 169, 92, 182]</t>
   </si>
   <si>
-    <t>[92, 183, 182, 46, 48, 188, 204, 206]</t>
+    <t>[92, 183, 182, 46, 188, 204, 48, 206]</t>
   </si>
   <si>
     <t>[89, 129, 105, 47]</t>
@@ -340,16 +340,16 @@
     <t>[88, 106, 104, 89, 47]</t>
   </si>
   <si>
-    <t>[87, 86, 88, 84, 44, 91, 105, 47, 83]</t>
-  </si>
-  <si>
-    <t>[109, 123, 2, 121, 127, 91, 90, 128]</t>
-  </si>
-  <si>
-    <t>[108, 123, 110, 2, 176]</t>
-  </si>
-  <si>
-    <t>[43, 122, 123, 126, 109, 176]</t>
+    <t>[87, 88, 84, 83, 86, 105, 47, 44, 91]</t>
+  </si>
+  <si>
+    <t>[127, 128, 2, 90, 109, 91, 123, 121]</t>
+  </si>
+  <si>
+    <t>[2, 176, 108, 110, 123]</t>
+  </si>
+  <si>
+    <t>[126, 176, 109, 122, 43, 123]</t>
   </si>
   <si>
     <t>[116, 99, 98, 100, 129]</t>
@@ -370,145 +370,145 @@
     <t>[95, 169, 93, 114, 185, 113]</t>
   </si>
   <si>
-    <t>[29, 64, 49, 119, 120]</t>
-  </si>
-  <si>
-    <t>[64, 67, 118, 154, 120, 157]</t>
-  </si>
-  <si>
-    <t>[118, 49, 144, 119, 205, 142, 157]</t>
-  </si>
-  <si>
-    <t>[122, 108, 123, 91]</t>
-  </si>
-  <si>
-    <t>[43, 44, 110, 123, 91, 121]</t>
-  </si>
-  <si>
-    <t>[122, 108, 110, 109, 121]</t>
-  </si>
-  <si>
-    <t>[81, 125, 126, 79]</t>
-  </si>
-  <si>
-    <t>[78, 177, 176, 126, 79, 124]</t>
-  </si>
-  <si>
-    <t>[43, 204, 110, 81, 125, 176, 124]</t>
-  </si>
-  <si>
-    <t>[356, 80, 287, 286, 108, 128, 291, 69, 2]</t>
-  </si>
-  <si>
-    <t>[72, 80, 130, 108, 127, 90]</t>
+    <t>[29, 119, 49, 120, 64]</t>
+  </si>
+  <si>
+    <t>[120, 157, 154, 67, 64, 118]</t>
+  </si>
+  <si>
+    <t>[119, 118, 49, 142, 157, 205, 144]</t>
+  </si>
+  <si>
+    <t>[108, 122, 123, 91]</t>
+  </si>
+  <si>
+    <t>[43, 110, 123, 121, 91, 44]</t>
+  </si>
+  <si>
+    <t>[109, 108, 122, 110, 121]</t>
+  </si>
+  <si>
+    <t>[125, 126, 79, 81]</t>
+  </si>
+  <si>
+    <t>[124, 126, 176, 78, 79, 177]</t>
+  </si>
+  <si>
+    <t>[124, 204, 43, 110, 125, 176, 81]</t>
+  </si>
+  <si>
+    <t>[356, 80, 287, 291, 286, 128, 69, 2, 108]</t>
+  </si>
+  <si>
+    <t>[80, 72, 127, 130, 90, 108]</t>
   </si>
   <si>
     <t>[93, 101, 72, 111, 98, 100, 130, 104, 89, 47]</t>
   </si>
   <si>
-    <t>[72, 88, 129, 128, 90, 89]</t>
-  </si>
-  <si>
-    <t>[19, 16, 17, 12, 132, 138, 77]</t>
-  </si>
-  <si>
-    <t>[138, 131, 140, 77]</t>
-  </si>
-  <si>
-    <t>[135, 199, 15, 18, 10, 17, 12, 138, 14]</t>
-  </si>
-  <si>
-    <t>[8, 139, 135, 137, 15, 14]</t>
-  </si>
-  <si>
-    <t>[139, 136, 16, 15]</t>
-  </si>
-  <si>
-    <t>[18, 17, 133, 132, 140, 131]</t>
-  </si>
-  <si>
-    <t>[11, 8, 19, 136, 137, 16]</t>
-  </si>
-  <si>
-    <t>[18, 26, 10, 132, 138, 77]</t>
-  </si>
-  <si>
-    <t>[465, 5, 145, 154, 143]</t>
-  </si>
-  <si>
-    <t>[144, 120, 145, 157, 143]</t>
-  </si>
-  <si>
-    <t>[465, 144, 145, 141, 142]</t>
-  </si>
-  <si>
-    <t>[465, 205, 143, 142, 120]</t>
-  </si>
-  <si>
-    <t>[141, 154, 157, 142, 143]</t>
-  </si>
-  <si>
-    <t>[147, 148, 29, 151, 64]</t>
-  </si>
-  <si>
-    <t>[151, 146, 150, 58, 148]</t>
-  </si>
-  <si>
-    <t>[147, 146, 58, 64]</t>
-  </si>
-  <si>
-    <t>[150, 27, 58, 64]</t>
-  </si>
-  <si>
-    <t>[152, 28, 147, 151, 27, 149, 63, 58]</t>
-  </si>
-  <si>
-    <t>[152, 147, 150, 29, 146, 63]</t>
-  </si>
-  <si>
-    <t>[151, 63, 150]</t>
-  </si>
-  <si>
-    <t>[155, 174, 173, 5, 154, 11, 76, 8]</t>
-  </si>
-  <si>
-    <t>[67, 119, 155, 65, 5, 153, 145, 141, 157]</t>
-  </si>
-  <si>
-    <t>[156, 65, 154, 153, 11]</t>
-  </si>
-  <si>
-    <t>[11, 155, 77, 9, 65]</t>
-  </si>
-  <si>
-    <t>[119, 120, 145, 154, 142]</t>
-  </si>
-  <si>
-    <t>[162, 159, 244, 197, 213, 216, 41]</t>
-  </si>
-  <si>
-    <t>[162, 160, 244, 158]</t>
-  </si>
-  <si>
-    <t>[162, 159, 244]</t>
-  </si>
-  <si>
-    <t>[212, 163, 164, 280, 262, 165]</t>
-  </si>
-  <si>
-    <t>[213, 158, 159, 160, 163, 164, 165, 244]</t>
-  </si>
-  <si>
-    <t>[161, 162, 213, 212, 164]</t>
-  </si>
-  <si>
-    <t>[161, 162, 163, 165]</t>
-  </si>
-  <si>
-    <t>[243, 161, 262, 162, 164, 244]</t>
-  </si>
-  <si>
-    <t>[82, 465, 184, 205, 5, 78]</t>
+    <t>[72, 128, 88, 129, 90, 89]</t>
+  </si>
+  <si>
+    <t>[19, 16, 77, 132, 17, 12, 138]</t>
+  </si>
+  <si>
+    <t>[77, 131, 140, 138]</t>
+  </si>
+  <si>
+    <t>[135, 199, 15, 74, 18, 17, 12, 138, 10, 14]</t>
+  </si>
+  <si>
+    <t>[135, 8, 137, 15, 139, 14]</t>
+  </si>
+  <si>
+    <t>[139, 16, 136, 15]</t>
+  </si>
+  <si>
+    <t>[132, 140, 18, 17, 131, 133]</t>
+  </si>
+  <si>
+    <t>[8, 137, 136, 19, 11, 16]</t>
+  </si>
+  <si>
+    <t>[26, 74, 77, 132, 18, 138, 10]</t>
+  </si>
+  <si>
+    <t>[5, 465, 143, 145, 154]</t>
+  </si>
+  <si>
+    <t>[120, 157, 144, 145, 143]</t>
+  </si>
+  <si>
+    <t>[142, 144, 141, 465, 145]</t>
+  </si>
+  <si>
+    <t>[142, 120, 205, 143, 465]</t>
+  </si>
+  <si>
+    <t>[142, 157, 141, 143, 154]</t>
+  </si>
+  <si>
+    <t>[29, 147, 151, 64, 148]</t>
+  </si>
+  <si>
+    <t>[58, 150, 151, 146, 148]</t>
+  </si>
+  <si>
+    <t>[147, 58, 146, 64]</t>
+  </si>
+  <si>
+    <t>[27, 150, 64, 58]</t>
+  </si>
+  <si>
+    <t>[27, 149, 28, 152, 63, 147, 58, 151]</t>
+  </si>
+  <si>
+    <t>[29, 152, 63, 147, 150, 146]</t>
+  </si>
+  <si>
+    <t>[150, 63, 151]</t>
+  </si>
+  <si>
+    <t>[5, 154, 174, 76, 173, 155, 8, 11]</t>
+  </si>
+  <si>
+    <t>[119, 67, 157, 141, 5, 145, 65, 153, 155]</t>
+  </si>
+  <si>
+    <t>[154, 65, 153, 156, 11]</t>
+  </si>
+  <si>
+    <t>[65, 155, 9, 11, 77]</t>
+  </si>
+  <si>
+    <t>[119, 142, 120, 154, 145]</t>
+  </si>
+  <si>
+    <t>[197, 159, 216, 244, 162, 213, 41]</t>
+  </si>
+  <si>
+    <t>[158, 162, 160, 244]</t>
+  </si>
+  <si>
+    <t>[159, 162, 244]</t>
+  </si>
+  <si>
+    <t>[163, 165, 164, 280, 262, 212]</t>
+  </si>
+  <si>
+    <t>[163, 165, 164, 159, 158, 213, 244, 160]</t>
+  </si>
+  <si>
+    <t>[212, 161, 213, 162, 164]</t>
+  </si>
+  <si>
+    <t>[163, 165, 161, 162]</t>
+  </si>
+  <si>
+    <t>[164, 161, 262, 243, 244, 162]</t>
+  </si>
+  <si>
+    <t>[82, 5, 465, 78, 184, 205]</t>
   </si>
   <si>
     <t>[168, 171, 237, 170, 102, 92]</t>
@@ -526,34 +526,34 @@
     <t>[102, 167, 170, 169]</t>
   </si>
   <si>
-    <t>[174, 6, 5, 180, 175, 179]</t>
-  </si>
-  <si>
-    <t>[13, 35, 52, 174, 6, 267, 153, 76]</t>
-  </si>
-  <si>
-    <t>[6, 172, 173, 5, 153]</t>
-  </si>
-  <si>
-    <t>[69, 82, 184, 2, 5, 180, 181, 172]</t>
-  </si>
-  <si>
-    <t>[110, 2, 109, 125, 177, 126]</t>
-  </si>
-  <si>
-    <t>[184, 2, 125, 78, 176]</t>
-  </si>
-  <si>
-    <t>[69, 290, 180, 181, 4]</t>
-  </si>
-  <si>
-    <t>[6, 180, 172, 4]</t>
-  </si>
-  <si>
-    <t>[181, 175, 172, 179, 178, 4]</t>
-  </si>
-  <si>
-    <t>[69, 180, 178, 175]</t>
+    <t>[5, 179, 175, 174, 6, 180]</t>
+  </si>
+  <si>
+    <t>[174, 6, 76, 13, 35, 52, 267, 153]</t>
+  </si>
+  <si>
+    <t>[5, 172, 6, 153, 173]</t>
+  </si>
+  <si>
+    <t>[82, 2, 5, 184, 172, 181, 180, 69]</t>
+  </si>
+  <si>
+    <t>[126, 2, 177, 110, 125, 109]</t>
+  </si>
+  <si>
+    <t>[2, 176, 78, 125, 184]</t>
+  </si>
+  <si>
+    <t>[290, 4, 181, 180, 69]</t>
+  </si>
+  <si>
+    <t>[4, 6, 172, 180]</t>
+  </si>
+  <si>
+    <t>[4, 179, 172, 181, 178, 175]</t>
+  </si>
+  <si>
+    <t>[180, 175, 178, 69]</t>
   </si>
   <si>
     <t>[102, 169, 92, 183, 185, 188, 103]</t>
@@ -562,7 +562,7 @@
     <t>[188, 182, 103]</t>
   </si>
   <si>
-    <t>[82, 175, 2, 166, 177, 78]</t>
+    <t>[82, 2, 78, 177, 175, 166]</t>
   </si>
   <si>
     <t>[169, 117, 182, 187, 113, 188]</t>
@@ -574,115 +574,115 @@
     <t>[188, 185, 186, 113]</t>
   </si>
   <si>
-    <t>[183, 182, 187, 185, 186, 103, 204, 45, 99, 85]</t>
-  </si>
-  <si>
-    <t>[191, 190, 192, 68, 195, 197, 196]</t>
-  </si>
-  <si>
-    <t>[191, 68, 195, 189]</t>
-  </si>
-  <si>
-    <t>[189, 68, 190]</t>
-  </si>
-  <si>
-    <t>[193, 189, 68, 197]</t>
-  </si>
-  <si>
-    <t>[68, 194, 192, 197]</t>
-  </si>
-  <si>
-    <t>[28, 193, 68, 27, 197, 64]</t>
-  </si>
-  <si>
-    <t>[190, 68, 66, 189, 25, 196]</t>
-  </si>
-  <si>
-    <t>[195, 197, 189, 25, 216, 22]</t>
-  </si>
-  <si>
-    <t>[28, 193, 192, 247, 194, 244, 189, 158, 216, 196]</t>
-  </si>
-  <si>
-    <t>[20, 21, 200, 26, 10]</t>
-  </si>
-  <si>
-    <t>[268, 201, 203, 267, 200, 135, 10, 133, 14]</t>
-  </si>
-  <si>
-    <t>[202, 22, 201, 21, 199, 198, 10]</t>
-  </si>
-  <si>
-    <t>[202, 203, 199, 200]</t>
-  </si>
-  <si>
-    <t>[200, 22, 201, 203, 216, 211]</t>
-  </si>
-  <si>
-    <t>[268, 202, 201, 211, 199]</t>
-  </si>
-  <si>
-    <t>[103, 188, 43, 33, 206, 45, 44, 126, 81]</t>
-  </si>
-  <si>
-    <t>[34, 30, 465, 49, 144, 120, 166, 467, 78]</t>
-  </si>
-  <si>
-    <t>[48, 103, 33, 50, 204]</t>
-  </si>
-  <si>
-    <t>[208, 279, 280, 281, 275, 209]</t>
-  </si>
-  <si>
-    <t>[271, 281, 207, 209, 246, 210]</t>
-  </si>
-  <si>
-    <t>[274, 208, 246, 279, 207, 269, 245, 210]</t>
-  </si>
-  <si>
-    <t>[208, 209, 274, 341, 346, 272, 271]</t>
-  </si>
-  <si>
-    <t>[3, 264, 268, 265, 38, 39, 37, 202, 203, 216]</t>
-  </si>
-  <si>
-    <t>[275, 161, 280, 163, 94, 245, 213, 266, 276, 278]</t>
-  </si>
-  <si>
-    <t>[162, 163, 212, 266, 158, 265, 41]</t>
-  </si>
-  <si>
-    <t>[460, 256, 255, 391, 343, 461, 248, 390, 346]</t>
-  </si>
-  <si>
-    <t>[255, 258, 249, 259, 218]</t>
-  </si>
-  <si>
-    <t>[197, 196, 158, 39, 41, 202, 22, 211]</t>
-  </si>
-  <si>
-    <t>[462, 221, 232, 463, 222, 225]</t>
-  </si>
-  <si>
-    <t>[460, 255, 249, 215, 224]</t>
-  </si>
-  <si>
-    <t>[249, 224, 223, 259]</t>
-  </si>
-  <si>
-    <t>[61, 466, 252, 227, 251]</t>
+    <t>[183, 182, 187, 185, 103, 186, 204, 45, 99, 85]</t>
+  </si>
+  <si>
+    <t>[192, 197, 191, 196, 68, 190, 195]</t>
+  </si>
+  <si>
+    <t>[191, 189, 68, 195]</t>
+  </si>
+  <si>
+    <t>[189, 190, 68]</t>
+  </si>
+  <si>
+    <t>[68, 193, 189, 197]</t>
+  </si>
+  <si>
+    <t>[194, 192, 197, 68]</t>
+  </si>
+  <si>
+    <t>[27, 28, 64, 197, 193, 68]</t>
+  </si>
+  <si>
+    <t>[189, 190, 68, 196, 66, 25]</t>
+  </si>
+  <si>
+    <t>[197, 189, 216, 195, 22, 25]</t>
+  </si>
+  <si>
+    <t>[247, 28, 194, 192, 193, 244, 158, 216, 196, 189]</t>
+  </si>
+  <si>
+    <t>[21, 20, 26, 200, 74, 10]</t>
+  </si>
+  <si>
+    <t>[201, 268, 267, 203, 135, 200, 133, 74, 10, 14]</t>
+  </si>
+  <si>
+    <t>[202, 201, 22, 21, 198, 199, 74, 10]</t>
+  </si>
+  <si>
+    <t>[202, 203, 200, 199]</t>
+  </si>
+  <si>
+    <t>[216, 22, 200, 211, 203, 201]</t>
+  </si>
+  <si>
+    <t>[202, 201, 268, 211, 199]</t>
+  </si>
+  <si>
+    <t>[103, 188, 206, 45, 44, 33, 43, 126, 81]</t>
+  </si>
+  <si>
+    <t>[49, 34, 30, 120, 144, 465, 78, 79, 166]</t>
+  </si>
+  <si>
+    <t>[103, 48, 50, 204, 33]</t>
+  </si>
+  <si>
+    <t>[208, 280, 281, 279, 209, 275]</t>
+  </si>
+  <si>
+    <t>[271, 210, 209, 281, 207]</t>
+  </si>
+  <si>
+    <t>[208, 210, 279, 207, 245, 269, 274]</t>
+  </si>
+  <si>
+    <t>[271, 272, 208, 346, 209, 341, 274]</t>
+  </si>
+  <si>
+    <t>[216, 265, 38, 39, 37, 202, 264, 268, 203, 3]</t>
+  </si>
+  <si>
+    <t>[276, 163, 161, 280, 213, 275, 94, 245, 266, 278]</t>
+  </si>
+  <si>
+    <t>[163, 158, 162, 212, 266, 41, 265]</t>
+  </si>
+  <si>
+    <t>[461, 390, 460, 256, 248, 255, 391, 346, 343]</t>
+  </si>
+  <si>
+    <t>[258, 255, 259, 218, 249]</t>
+  </si>
+  <si>
+    <t>[197, 158, 41, 39, 196, 22, 202, 211]</t>
+  </si>
+  <si>
+    <t>[462, 221, 463, 232, 222, 225]</t>
+  </si>
+  <si>
+    <t>[460, 224, 215, 255, 249]</t>
+  </si>
+  <si>
+    <t>[259, 223, 224, 249]</t>
+  </si>
+  <si>
+    <t>[61, 252, 227, 466]</t>
   </si>
   <si>
     <t>[462, 232, 250, 217]</t>
   </si>
   <si>
-    <t>[217, 463, 225, 224, 460, 459]</t>
-  </si>
-  <si>
-    <t>[219, 259, 224, 226, 241, 225]</t>
-  </si>
-  <si>
-    <t>[222, 460, 249, 219, 218, 225, 223]</t>
+    <t>[463, 217, 459, 225, 224, 460]</t>
+  </si>
+  <si>
+    <t>[219, 224, 226, 241, 225, 259]</t>
+  </si>
+  <si>
+    <t>[222, 460, 219, 225, 223, 218, 249]</t>
   </si>
   <si>
     <t>[217, 222, 224, 226, 232, 223]</t>
@@ -697,13 +697,13 @@
     <t>[237, 62, 61, 226, 232, 236]</t>
   </si>
   <si>
-    <t>[248, 230, 36, 273, 272, 231]</t>
+    <t>[248, 230, 231, 36, 272, 273]</t>
   </si>
   <si>
     <t>[231, 36, 229]</t>
   </si>
   <si>
-    <t>[282, 238, 230, 36, 273, 229, 281]</t>
+    <t>[282, 238, 230, 36, 281, 273, 229]</t>
   </si>
   <si>
     <t>[221, 250, 237, 217, 226, 228, 225]</t>
@@ -724,223 +724,223 @@
     <t>[167, 250, 232, 92, 62, 228]</t>
   </si>
   <si>
-    <t>[282, 240, 239, 231, 281, 262]</t>
-  </si>
-  <si>
-    <t>[252, 254, 240, 238, 263, 262]</t>
-  </si>
-  <si>
-    <t>[254, 282, 259, 226, 233, 239, 241, 238]</t>
-  </si>
-  <si>
-    <t>[259, 226, 240, 223]</t>
-  </si>
-  <si>
-    <t>[260, 263, 251, 253, 247, 243]</t>
-  </si>
-  <si>
-    <t>[242, 247, 260, 244, 165, 262]</t>
-  </si>
-  <si>
-    <t>[247, 243, 162, 159, 160, 165, 197, 158]</t>
-  </si>
-  <si>
-    <t>[279, 275, 209, 94, 269, 212]</t>
-  </si>
-  <si>
-    <t>[61, 466, 28, 242, 253, 197, 244, 243]</t>
-  </si>
-  <si>
-    <t>[256, 214, 36, 346, 272, 229]</t>
-  </si>
-  <si>
-    <t>[219, 259, 215, 218, 224]</t>
+    <t>[239, 282, 262, 281, 231, 240]</t>
+  </si>
+  <si>
+    <t>[252, 254, 262, 238, 263, 240]</t>
+  </si>
+  <si>
+    <t>[254, 239, 282, 238, 226, 233, 259, 241]</t>
+  </si>
+  <si>
+    <t>[226, 240, 259, 223]</t>
+  </si>
+  <si>
+    <t>[253, 251, 247, 261, 263, 243, 260]</t>
+  </si>
+  <si>
+    <t>[247, 261, 242, 165, 262, 244, 260]</t>
+  </si>
+  <si>
+    <t>[247, 197, 165, 243, 159, 158, 162, 160]</t>
+  </si>
+  <si>
+    <t>[279, 209, 275, 94, 269, 212]</t>
+  </si>
+  <si>
+    <t>[61, 466, 253, 28, 242, 243, 244, 197]</t>
+  </si>
+  <si>
+    <t>[256, 214, 36, 229, 272, 346]</t>
+  </si>
+  <si>
+    <t>[219, 224, 215, 259, 218]</t>
   </si>
   <si>
     <t>[462, 221, 237, 232]</t>
   </si>
   <si>
-    <t>[466, 252, 220, 242, 253, 263]</t>
-  </si>
-  <si>
-    <t>[263, 251, 220, 239, 254, 227]</t>
-  </si>
-  <si>
-    <t>[466, 242, 251, 247]</t>
+    <t>[252, 466, 253, 263, 242]</t>
+  </si>
+  <si>
+    <t>[251, 263, 239, 254, 220, 227, 466]</t>
+  </si>
+  <si>
+    <t>[466, 247, 251, 242]</t>
   </si>
   <si>
     <t>[252, 227, 233, 239, 240]</t>
   </si>
   <si>
-    <t>[460, 256, 257, 214, 218, 258, 215]</t>
-  </si>
-  <si>
-    <t>[255, 214, 257, 36, 248]</t>
-  </si>
-  <si>
-    <t>[256, 282, 36, 259, 255, 258]</t>
-  </si>
-  <si>
-    <t>[257, 255, 259, 215]</t>
-  </si>
-  <si>
-    <t>[282, 257, 258, 249, 219, 241, 223, 240, 215]</t>
-  </si>
-  <si>
-    <t>[242, 263, 243, 262]</t>
-  </si>
-  <si>
-    <t>[260, 243, 238, 239, 263, 281, 161, 280, 165]</t>
-  </si>
-  <si>
-    <t>[252, 242, 251, 260, 239, 262]</t>
-  </si>
-  <si>
-    <t>[3, 211, 266, 265]</t>
-  </si>
-  <si>
-    <t>[264, 266, 213, 211, 37, 41, 40]</t>
-  </si>
-  <si>
-    <t>[380, 3, 57, 212, 276, 264, 379, 213, 277, 265]</t>
-  </si>
-  <si>
-    <t>[3, 54, 52, 173, 268, 199, 76, 135, 14]</t>
-  </si>
-  <si>
-    <t>[3, 211, 267, 199, 203]</t>
-  </si>
-  <si>
-    <t>[274, 209, 354, 94, 270, 245, 278]</t>
-  </si>
-  <si>
-    <t>[333, 378, 338, 354, 269, 278, 385, 277, 332]</t>
-  </si>
-  <si>
-    <t>[208, 246, 273, 272, 281, 210]</t>
-  </si>
-  <si>
-    <t>[248, 246, 273, 229, 271, 346, 210]</t>
-  </si>
-  <si>
-    <t>[229, 231, 271, 281, 272]</t>
-  </si>
-  <si>
-    <t>[345, 341, 246, 348, 355, 354, 209, 269, 210]</t>
-  </si>
-  <si>
-    <t>[279, 207, 212, 245, 280]</t>
-  </si>
-  <si>
-    <t>[212, 278, 266, 277]</t>
-  </si>
-  <si>
-    <t>[278, 270, 276, 266, 382, 379, 385]</t>
-  </si>
-  <si>
-    <t>[94, 269, 212, 276, 270, 277]</t>
-  </si>
-  <si>
-    <t>[207, 275, 209, 245]</t>
-  </si>
-  <si>
-    <t>[207, 275, 281, 161, 212, 262]</t>
-  </si>
-  <si>
-    <t>[238, 208, 207, 273, 231, 271, 262, 280]</t>
-  </si>
-  <si>
-    <t>[257, 36, 259, 240, 238, 231]</t>
-  </si>
-  <si>
-    <t>[285, 57, 0, 55, 1]</t>
-  </si>
-  <si>
-    <t>[288, 380, 285, 289, 57]</t>
-  </si>
-  <si>
-    <t>[289, 284, 57, 283, 1]</t>
-  </si>
-  <si>
-    <t>[388, 324, 287, 291, 294, 455, 127]</t>
-  </si>
-  <si>
-    <t>[454, 456, 356, 455, 286, 127]</t>
-  </si>
-  <si>
-    <t>[325, 327, 284, 380, 289, 383, 381]</t>
-  </si>
-  <si>
-    <t>[325, 388, 324, 288, 285, 284, 7, 1]</t>
-  </si>
-  <si>
-    <t>[292, 69, 178, 7, 4]</t>
-  </si>
-  <si>
-    <t>[388, 286, 127, 292, 69, 7]</t>
-  </si>
-  <si>
-    <t>[69, 291, 290, 7]</t>
-  </si>
-  <si>
-    <t>[298, 328, 330, 312, 299, 302]</t>
-  </si>
-  <si>
-    <t>[324, 328, 312, 286, 455, 315, 297]</t>
-  </si>
-  <si>
-    <t>[454, 323, 305, 296, 300, 455]</t>
-  </si>
-  <si>
-    <t>[321, 300, 297, 295, 455]</t>
-  </si>
-  <si>
-    <t>[294, 296, 455, 320, 321, 315]</t>
-  </si>
-  <si>
-    <t>[299, 293, 330]</t>
-  </si>
-  <si>
-    <t>[308, 309, 307, 298, 330, 293, 311, 302]</t>
-  </si>
-  <si>
-    <t>[323, 322, 296, 306, 295, 321]</t>
-  </si>
-  <si>
-    <t>[312, 302, 303, 314, 313, 315, 317]</t>
-  </si>
-  <si>
-    <t>[293, 299, 312, 303, 311, 301]</t>
-  </si>
-  <si>
-    <t>[302, 311, 301, 304, 313]</t>
-  </si>
-  <si>
-    <t>[311, 310, 303, 314, 313, 318, 306, 319, 316]</t>
-  </si>
-  <si>
-    <t>[454, 323, 392, 322, 295]</t>
-  </si>
-  <si>
-    <t>[322, 310, 300, 304, 320, 321, 319]</t>
-  </si>
-  <si>
-    <t>[308, 371, 364, 358, 299, 330, 359]</t>
+    <t>[460, 256, 257, 215, 258, 218, 214]</t>
+  </si>
+  <si>
+    <t>[257, 255, 214, 248, 36]</t>
+  </si>
+  <si>
+    <t>[282, 256, 259, 36, 258, 255]</t>
+  </si>
+  <si>
+    <t>[257, 215, 255, 259]</t>
+  </si>
+  <si>
+    <t>[282, 219, 257, 240, 241, 223, 215, 258, 249]</t>
+  </si>
+  <si>
+    <t>[262, 243, 242, 263]</t>
+  </si>
+  <si>
+    <t>[239, 238, 261, 263, 165, 161, 281, 280, 243, 260]</t>
+  </si>
+  <si>
+    <t>[252, 251, 239, 261, 242, 262, 260]</t>
+  </si>
+  <si>
+    <t>[265, 266, 211, 3]</t>
+  </si>
+  <si>
+    <t>[213, 40, 41, 266, 264, 211, 37]</t>
+  </si>
+  <si>
+    <t>[379, 276, 213, 380, 212, 265, 264, 277, 57, 3]</t>
+  </si>
+  <si>
+    <t>[76, 52, 173, 268, 135, 199, 54, 3, 14]</t>
+  </si>
+  <si>
+    <t>[3, 211, 267, 203, 199]</t>
+  </si>
+  <si>
+    <t>[209, 94, 245, 274, 354, 278, 270]</t>
+  </si>
+  <si>
+    <t>[269, 278, 354, 277, 385, 333, 338, 378, 332]</t>
+  </si>
+  <si>
+    <t>[273, 281, 208, 210, 272]</t>
+  </si>
+  <si>
+    <t>[248, 229, 271, 273, 346, 210]</t>
+  </si>
+  <si>
+    <t>[231, 229, 271, 281, 272]</t>
+  </si>
+  <si>
+    <t>[210, 341, 345, 209, 355, 269, 348, 354]</t>
+  </si>
+  <si>
+    <t>[280, 279, 212, 207, 245]</t>
+  </si>
+  <si>
+    <t>[266, 277, 212, 278]</t>
+  </si>
+  <si>
+    <t>[379, 276, 266, 278, 382, 270, 385]</t>
+  </si>
+  <si>
+    <t>[276, 94, 212, 269, 277, 270]</t>
+  </si>
+  <si>
+    <t>[245, 209, 275, 207]</t>
+  </si>
+  <si>
+    <t>[161, 262, 281, 212, 275, 207]</t>
+  </si>
+  <si>
+    <t>[238, 231, 262, 271, 273, 208, 280, 207]</t>
+  </si>
+  <si>
+    <t>[257, 259, 36, 231, 238, 240]</t>
+  </si>
+  <si>
+    <t>[285, 1, 57, 55, 0]</t>
+  </si>
+  <si>
+    <t>[288, 289, 285, 380, 57]</t>
+  </si>
+  <si>
+    <t>[289, 1, 284, 283, 57]</t>
+  </si>
+  <si>
+    <t>[388, 287, 291, 127, 294, 324, 455]</t>
+  </si>
+  <si>
+    <t>[356, 456, 127, 286, 455, 454]</t>
+  </si>
+  <si>
+    <t>[327, 467, 289, 383, 284, 380, 381]</t>
+  </si>
+  <si>
+    <t>[325, 467, 288, 324, 388, 1, 285, 284, 7]</t>
+  </si>
+  <si>
+    <t>[7, 292, 4, 69, 178]</t>
+  </si>
+  <si>
+    <t>[388, 286, 127, 7, 292, 69]</t>
+  </si>
+  <si>
+    <t>[291, 290, 7, 69]</t>
+  </si>
+  <si>
+    <t>[328, 302, 312, 298, 330, 299]</t>
+  </si>
+  <si>
+    <t>[297, 315, 455, 286, 324, 328, 312]</t>
+  </si>
+  <si>
+    <t>[454, 305, 455, 300, 323, 296]</t>
+  </si>
+  <si>
+    <t>[297, 455, 300, 295, 321]</t>
+  </si>
+  <si>
+    <t>[294, 320, 315, 455, 321, 296]</t>
+  </si>
+  <si>
+    <t>[293, 330, 299]</t>
+  </si>
+  <si>
+    <t>[309, 308, 307, 302, 311, 298, 293, 330]</t>
+  </si>
+  <si>
+    <t>[323, 295, 296, 321, 306, 322]</t>
+  </si>
+  <si>
+    <t>[315, 302, 312, 303, 314, 313, 317]</t>
+  </si>
+  <si>
+    <t>[312, 293, 299, 311, 303, 301]</t>
+  </si>
+  <si>
+    <t>[302, 311, 304, 313, 301]</t>
+  </si>
+  <si>
+    <t>[310, 318, 319, 311, 303, 314, 306, 313, 316]</t>
+  </si>
+  <si>
+    <t>[392, 454, 322, 295, 323]</t>
+  </si>
+  <si>
+    <t>[310, 320, 319, 304, 300, 321, 322]</t>
+  </si>
+  <si>
+    <t>[359, 358, 371, 364, 308, 330, 299]</t>
   </si>
   <si>
     <t>[364, 309, 307, 299]</t>
   </si>
   <si>
-    <t>[308, 366, 364, 310, 311, 367, 299]</t>
-  </si>
-  <si>
-    <t>[309, 322, 392, 412, 367, 311, 396, 306, 304]</t>
-  </si>
-  <si>
-    <t>[309, 299, 302, 310, 303, 304]</t>
-  </si>
-  <si>
-    <t>[328, 293, 294, 315, 302, 301]</t>
+    <t>[310, 364, 366, 367, 311, 308, 299]</t>
+  </si>
+  <si>
+    <t>[412, 392, 396, 367, 322, 306, 304, 311, 309]</t>
+  </si>
+  <si>
+    <t>[310, 309, 302, 304, 303, 299]</t>
+  </si>
+  <si>
+    <t>[294, 328, 315, 302, 293, 301]</t>
   </si>
   <si>
     <t>[303, 314, 304, 301]</t>
@@ -949,238 +949,238 @@
     <t>[304, 316, 313, 301, 317]</t>
   </si>
   <si>
-    <t>[312, 294, 301, 317, 320, 319, 297]</t>
-  </si>
-  <si>
-    <t>[314, 318, 304, 317]</t>
-  </si>
-  <si>
-    <t>[314, 301, 318, 316, 315, 319]</t>
+    <t>[294, 320, 312, 301, 297, 317, 319]</t>
+  </si>
+  <si>
+    <t>[318, 314, 304, 317]</t>
+  </si>
+  <si>
+    <t>[315, 318, 319, 314, 316, 301]</t>
   </si>
   <si>
     <t>[304, 316, 319, 317]</t>
   </si>
   <si>
-    <t>[318, 304, 317, 320, 306, 315]</t>
-  </si>
-  <si>
-    <t>[321, 306, 319, 297, 315]</t>
-  </si>
-  <si>
-    <t>[296, 300, 320, 306, 297]</t>
-  </si>
-  <si>
-    <t>[323, 305, 392, 310, 306, 300]</t>
-  </si>
-  <si>
-    <t>[295, 305, 300, 322]</t>
-  </si>
-  <si>
-    <t>[325, 388, 328, 294, 357, 289, 286]</t>
-  </si>
-  <si>
-    <t>[324, 357, 327, 288, 289]</t>
-  </si>
-  <si>
-    <t>[363, 325, 288, 358, 357, 360, 373, 383]</t>
-  </si>
-  <si>
-    <t>[324, 329, 357, 294, 330, 293, 312]</t>
-  </si>
-  <si>
-    <t>[357, 328, 330, 359]</t>
-  </si>
-  <si>
-    <t>[307, 298, 329, 328, 299, 293, 359]</t>
-  </si>
-  <si>
-    <t>[362, 334, 360, 361, 337]</t>
-  </si>
-  <si>
-    <t>[386, 387, 338, 270, 378, 384]</t>
-  </si>
-  <si>
-    <t>[335, 362, 344, 336, 331, 337]</t>
-  </si>
-  <si>
-    <t>[342, 353, 362, 334, 352, 344]</t>
-  </si>
-  <si>
-    <t>[348, 344, 334, 360, 337, 355, 350, 351]</t>
-  </si>
-  <si>
-    <t>[334, 360, 331, 336]</t>
-  </si>
-  <si>
-    <t>[333, 339, 354, 270, 387, 332]</t>
-  </si>
-  <si>
-    <t>[387, 355, 338, 354]</t>
-  </si>
-  <si>
-    <t>[350, 349, 351, 346, 352]</t>
-  </si>
-  <si>
-    <t>[345, 246, 274, 346, 210]</t>
-  </si>
-  <si>
-    <t>[343, 335, 353, 346, 352]</t>
-  </si>
-  <si>
-    <t>[391, 214, 353, 342, 346]</t>
-  </si>
-  <si>
-    <t>[335, 336, 334, 352, 351]</t>
-  </si>
-  <si>
-    <t>[348, 347, 346, 341, 274]</t>
-  </si>
-  <si>
-    <t>[343, 214, 342, 248, 345, 341, 347, 246, 272, 340, 349, 352, 210]</t>
+    <t>[320, 315, 318, 304, 306, 317]</t>
+  </si>
+  <si>
+    <t>[297, 315, 319, 321, 306]</t>
+  </si>
+  <si>
+    <t>[320, 297, 300, 296, 306]</t>
+  </si>
+  <si>
+    <t>[392, 310, 305, 300, 323, 306]</t>
+  </si>
+  <si>
+    <t>[305, 300, 295, 322]</t>
+  </si>
+  <si>
+    <t>[325, 357, 289, 388, 294, 286, 328]</t>
+  </si>
+  <si>
+    <t>[289, 467, 324, 357]</t>
+  </si>
+  <si>
+    <t>[360, 373, 363, 383, 358, 288, 467, 357]</t>
+  </si>
+  <si>
+    <t>[357, 329, 294, 324, 330, 293, 312]</t>
+  </si>
+  <si>
+    <t>[359, 357, 328, 330]</t>
+  </si>
+  <si>
+    <t>[359, 329, 328, 307, 298, 293, 299]</t>
+  </si>
+  <si>
+    <t>[361, 362, 337, 334, 360]</t>
+  </si>
+  <si>
+    <t>[384, 386, 378, 270, 338, 387]</t>
+  </si>
+  <si>
+    <t>[335, 362, 344, 337, 336, 331]</t>
+  </si>
+  <si>
+    <t>[342, 353, 352, 334, 362, 344]</t>
+  </si>
+  <si>
+    <t>[355, 348, 351, 344, 350, 337, 360, 334]</t>
+  </si>
+  <si>
+    <t>[336, 334, 331, 360]</t>
+  </si>
+  <si>
+    <t>[354, 339, 333, 270, 387, 332]</t>
+  </si>
+  <si>
+    <t>[355, 354, 387, 338]</t>
+  </si>
+  <si>
+    <t>[349, 346, 351, 352, 350]</t>
+  </si>
+  <si>
+    <t>[210, 346, 345, 274]</t>
+  </si>
+  <si>
+    <t>[343, 346, 352, 353, 335]</t>
+  </si>
+  <si>
+    <t>[214, 391, 346, 342, 353]</t>
+  </si>
+  <si>
+    <t>[335, 351, 352, 334, 336]</t>
+  </si>
+  <si>
+    <t>[341, 346, 347, 348, 274]</t>
+  </si>
+  <si>
+    <t>[248, 214, 272, 210, 341, 345, 343, 342, 349, 347, 352, 340]</t>
   </si>
   <si>
     <t>[345, 348, 349, 346, 350]</t>
   </si>
   <si>
-    <t>[345, 274, 355, 336, 347, 350]</t>
-  </si>
-  <si>
-    <t>[347, 340, 350, 346]</t>
-  </si>
-  <si>
-    <t>[348, 347, 336, 340, 349, 351]</t>
-  </si>
-  <si>
-    <t>[344, 336, 340, 350, 352]</t>
-  </si>
-  <si>
-    <t>[335, 342, 344, 340, 351, 346]</t>
-  </si>
-  <si>
-    <t>[391, 343, 335, 342, 362, 458]</t>
-  </si>
-  <si>
-    <t>[274, 339, 338, 355, 269, 270]</t>
-  </si>
-  <si>
-    <t>[274, 348, 339, 354, 360, 387, 336]</t>
-  </si>
-  <si>
-    <t>[456, 405, 394, 80, 287, 127]</t>
-  </si>
-  <si>
-    <t>[325, 324, 358, 329, 328, 327, 359]</t>
-  </si>
-  <si>
-    <t>[363, 371, 307, 327, 357, 359]</t>
-  </si>
-  <si>
-    <t>[307, 358, 329, 357, 330]</t>
-  </si>
-  <si>
-    <t>[331, 361, 373, 337, 386, 387, 336, 327, 355, 383]</t>
-  </si>
-  <si>
-    <t>[374, 423, 362, 360, 331, 373]</t>
-  </si>
-  <si>
-    <t>[335, 353, 458, 457, 423, 334, 361, 331]</t>
-  </si>
-  <si>
-    <t>[371, 358, 374, 373, 375, 327]</t>
-  </si>
-  <si>
-    <t>[308, 366, 371, 307, 309]</t>
-  </si>
-  <si>
-    <t>[370, 412, 367, 372, 368]</t>
-  </si>
-  <si>
-    <t>[370, 371, 367, 364, 309, 368]</t>
-  </si>
-  <si>
-    <t>[366, 309, 370, 412, 310, 365, 368]</t>
-  </si>
-  <si>
-    <t>[365, 372, 376, 375, 371, 366, 367]</t>
-  </si>
-  <si>
-    <t>[363, 375, 366, 307, 358, 364, 370, 368]</t>
-  </si>
-  <si>
-    <t>[370, 412, 365, 376, 368]</t>
-  </si>
-  <si>
-    <t>[363, 374, 360, 361, 327]</t>
+    <t>[345, 355, 274, 350, 347, 336]</t>
+  </si>
+  <si>
+    <t>[346, 347, 340, 350]</t>
+  </si>
+  <si>
+    <t>[348, 349, 347, 351, 340, 336]</t>
+  </si>
+  <si>
+    <t>[340, 352, 344, 350, 336]</t>
+  </si>
+  <si>
+    <t>[342, 346, 335, 351, 340, 344]</t>
+  </si>
+  <si>
+    <t>[343, 391, 458, 342, 362, 335]</t>
+  </si>
+  <si>
+    <t>[355, 274, 269, 339, 270, 338]</t>
+  </si>
+  <si>
+    <t>[274, 354, 348, 339, 387, 336, 360]</t>
+  </si>
+  <si>
+    <t>[405, 80, 394, 456, 127, 287]</t>
+  </si>
+  <si>
+    <t>[325, 327, 467, 359, 358, 324, 328, 329]</t>
+  </si>
+  <si>
+    <t>[327, 363, 359, 307, 371, 357]</t>
+  </si>
+  <si>
+    <t>[307, 358, 330, 357, 329]</t>
+  </si>
+  <si>
+    <t>[327, 373, 355, 361, 337, 336, 331, 383, 386, 387]</t>
+  </si>
+  <si>
+    <t>[374, 423, 373, 362, 360, 331]</t>
+  </si>
+  <si>
+    <t>[457, 423, 458, 353, 335, 361, 334, 331]</t>
+  </si>
+  <si>
+    <t>[327, 371, 358, 374, 373, 375]</t>
+  </si>
+  <si>
+    <t>[371, 366, 307, 308, 309]</t>
+  </si>
+  <si>
+    <t>[412, 370, 372, 367, 368]</t>
+  </si>
+  <si>
+    <t>[370, 371, 364, 367, 309, 368]</t>
+  </si>
+  <si>
+    <t>[412, 370, 365, 310, 366, 309, 368]</t>
+  </si>
+  <si>
+    <t>[365, 367, 366, 371, 375, 376, 372]</t>
+  </si>
+  <si>
+    <t>[363, 358, 370, 307, 375, 364, 366, 368]</t>
+  </si>
+  <si>
+    <t>[412, 370, 365, 376, 368]</t>
+  </si>
+  <si>
+    <t>[327, 363, 374, 360, 361]</t>
   </si>
   <si>
     <t>[363, 375, 423, 373, 361]</t>
   </si>
   <si>
-    <t>[363, 423, 422, 376, 374, 371, 370, 368]</t>
-  </si>
-  <si>
-    <t>[375, 422, 370, 412, 411, 372, 368]</t>
-  </si>
-  <si>
-    <t>[381, 382, 379, 385]</t>
-  </si>
-  <si>
-    <t>[333, 383, 384, 385, 270, 332]</t>
-  </si>
-  <si>
-    <t>[380, 381, 266, 382, 377, 277]</t>
-  </si>
-  <si>
-    <t>[288, 284, 379, 266, 381, 57]</t>
-  </si>
-  <si>
-    <t>[288, 380, 383, 379, 385, 377]</t>
-  </si>
-  <si>
-    <t>[377, 379, 385, 277]</t>
-  </si>
-  <si>
-    <t>[288, 378, 384, 381, 360, 386, 327, 385]</t>
-  </si>
-  <si>
-    <t>[333, 378, 383, 386, 332]</t>
-  </si>
-  <si>
-    <t>[378, 381, 270, 383, 382, 377, 277]</t>
-  </si>
-  <si>
-    <t>[333, 384, 360, 383, 387, 332]</t>
-  </si>
-  <si>
-    <t>[333, 339, 338, 360, 386, 355, 332]</t>
-  </si>
-  <si>
-    <t>[291, 7, 289, 324, 286]</t>
-  </si>
-  <si>
-    <t>[458, 457, 390, 459, 461]</t>
-  </si>
-  <si>
-    <t>[391, 214, 389, 458, 461]</t>
-  </si>
-  <si>
-    <t>[353, 458, 343, 214, 390]</t>
-  </si>
-  <si>
-    <t>[454, 305, 322, 456, 310, 396, 394, 393]</t>
-  </si>
-  <si>
-    <t>[392, 394, 395, 396, 398, 399, 397]</t>
-  </si>
-  <si>
-    <t>[456, 405, 392, 401, 356, 393, 395]</t>
+    <t>[363, 422, 374, 423, 370, 376, 371, 368]</t>
+  </si>
+  <si>
+    <t>[411, 422, 412, 370, 372, 375, 368]</t>
+  </si>
+  <si>
+    <t>[379, 381, 382, 385]</t>
+  </si>
+  <si>
+    <t>[383, 385, 333, 270, 384, 332]</t>
+  </si>
+  <si>
+    <t>[382, 277, 377, 381, 380, 266]</t>
+  </si>
+  <si>
+    <t>[288, 379, 284, 381, 266, 57]</t>
+  </si>
+  <si>
+    <t>[288, 379, 380, 383, 377, 385]</t>
+  </si>
+  <si>
+    <t>[379, 377, 277, 385]</t>
+  </si>
+  <si>
+    <t>[327, 288, 360, 381, 386, 384, 385, 378]</t>
+  </si>
+  <si>
+    <t>[383, 333, 378, 386, 332]</t>
+  </si>
+  <si>
+    <t>[381, 377, 382, 277, 383, 270, 378]</t>
+  </si>
+  <si>
+    <t>[360, 383, 333, 384, 387, 332]</t>
+  </si>
+  <si>
+    <t>[355, 360, 339, 333, 338, 386, 332]</t>
+  </si>
+  <si>
+    <t>[289, 324, 286, 291, 7]</t>
+  </si>
+  <si>
+    <t>[457, 461, 390, 458, 459]</t>
+  </si>
+  <si>
+    <t>[461, 214, 391, 458, 389]</t>
+  </si>
+  <si>
+    <t>[390, 214, 343, 458, 353]</t>
+  </si>
+  <si>
+    <t>[310, 396, 322, 393, 305, 454, 456, 394]</t>
+  </si>
+  <si>
+    <t>[395, 392, 396, 394, 398, 399, 397]</t>
+  </si>
+  <si>
+    <t>[405, 356, 395, 392, 456, 401, 393]</t>
   </si>
   <si>
     <t>[394, 401, 393, 399]</t>
   </si>
   <si>
-    <t>[392, 412, 409, 310, 401, 393, 397]</t>
+    <t>[409, 412, 392, 401, 310, 397, 393]</t>
   </si>
   <si>
     <t>[396, 398, 401, 393]</t>
@@ -1192,40 +1192,40 @@
     <t>[395, 398, 401, 393]</t>
   </si>
   <si>
-    <t>[402, 405, 403, 394, 409, 395, 396, 398, 399, 397]</t>
-  </si>
-  <si>
-    <t>[404, 405, 401, 403, 409, 407]</t>
+    <t>[405, 403, 402, 409, 395, 396, 394, 398, 399, 397]</t>
+  </si>
+  <si>
+    <t>[405, 407, 404, 403, 401, 409]</t>
   </si>
   <si>
     <t>[402, 401, 409]</t>
   </si>
   <si>
-    <t>[464, 406, 402, 405, 407]</t>
-  </si>
-  <si>
-    <t>[464, 402, 404, 80, 356, 394, 401]</t>
-  </si>
-  <si>
-    <t>[464, 410, 404, 408, 407]</t>
-  </si>
-  <si>
-    <t>[406, 402, 404, 412, 409, 408]</t>
-  </si>
-  <si>
-    <t>[410, 406, 412, 452, 407, 442]</t>
-  </si>
-  <si>
-    <t>[402, 403, 412, 401, 396, 407]</t>
-  </si>
-  <si>
-    <t>[451, 464, 448, 447, 442, 406, 408]</t>
-  </si>
-  <si>
-    <t>[429, 422, 412, 452, 376]</t>
-  </si>
-  <si>
-    <t>[310, 367, 365, 396, 409, 452, 411, 372, 407, 376, 408]</t>
+    <t>[464, 405, 407, 406, 402]</t>
+  </si>
+  <si>
+    <t>[464, 402, 404, 356, 80, 401, 394]</t>
+  </si>
+  <si>
+    <t>[464, 407, 408, 410, 404]</t>
+  </si>
+  <si>
+    <t>[412, 408, 409, 402, 406, 404]</t>
+  </si>
+  <si>
+    <t>[407, 406, 410, 442, 452, 412]</t>
+  </si>
+  <si>
+    <t>[407, 403, 402, 396, 401, 412]</t>
+  </si>
+  <si>
+    <t>[451, 464, 408, 406, 442, 448, 447]</t>
+  </si>
+  <si>
+    <t>[429, 452, 412, 376, 422]</t>
+  </si>
+  <si>
+    <t>[407, 408, 409, 411, 452, 396, 376, 310, 372, 365, 367]</t>
   </si>
   <si>
     <t>[416, 421, 418, 420, 419, 417, 415]</t>
@@ -1249,148 +1249,148 @@
     <t>[417, 413, 414, 415]</t>
   </si>
   <si>
-    <t>[421, 418, 423, 457, 413, 414, 415]</t>
+    <t>[421, 457, 418, 423, 413, 414, 415]</t>
   </si>
   <si>
     <t>[416, 457, 420, 413]</t>
   </si>
   <si>
-    <t>[453, 375, 429, 438, 423, 376, 411]</t>
-  </si>
-  <si>
-    <t>[453, 375, 422, 418, 420, 457, 374, 362, 361]</t>
-  </si>
-  <si>
-    <t>[442, 440, 426, 443, 427, 445]</t>
-  </si>
-  <si>
-    <t>[453, 438, 437, 448, 436]</t>
-  </si>
-  <si>
-    <t>[444, 439, 443, 427, 424, 445]</t>
-  </si>
-  <si>
-    <t>[426, 443, 424]</t>
-  </si>
-  <si>
-    <t>[452, 411, 438, 422]</t>
+    <t>[429, 411, 453, 423, 375, 438, 376]</t>
+  </si>
+  <si>
+    <t>[457, 422, 453, 418, 420, 374, 375, 362, 361]</t>
+  </si>
+  <si>
+    <t>[428, 445, 426, 440, 443, 442, 427]</t>
+  </si>
+  <si>
+    <t>[453, 448, 437, 438, 436]</t>
+  </si>
+  <si>
+    <t>[439, 444, 428, 445, 443, 424, 427]</t>
+  </si>
+  <si>
+    <t>[426, 424, 443]</t>
+  </si>
+  <si>
+    <t>[411, 452, 438, 422]</t>
   </si>
   <si>
     <t>[450, 439, 444, 432, 431]</t>
   </si>
   <si>
-    <t>[444, 430, 433, 434, 432]</t>
+    <t>[430, 444, 433, 432, 434]</t>
   </si>
   <si>
     <t>[450, 430, 433, 431, 449]</t>
   </si>
   <si>
-    <t>[431, 434, 432, 449]</t>
-  </si>
-  <si>
-    <t>[435, 444, 433, 431, 449]</t>
-  </si>
-  <si>
-    <t>[437, 448, 436, 445, 449, 434, 444]</t>
-  </si>
-  <si>
-    <t>[438, 437, 425, 452, 445, 435]</t>
-  </si>
-  <si>
-    <t>[435, 448, 425, 436]</t>
-  </si>
-  <si>
-    <t>[453, 429, 422, 452, 436, 425]</t>
-  </si>
-  <si>
-    <t>[450, 441, 426, 430, 444, 443]</t>
-  </si>
-  <si>
-    <t>[442, 441, 424, 443]</t>
-  </si>
-  <si>
-    <t>[447, 450, 442, 440, 439, 443]</t>
-  </si>
-  <si>
-    <t>[410, 447, 452, 408, 445, 441, 424, 440]</t>
-  </si>
-  <si>
-    <t>[440, 441, 426, 439, 424, 427]</t>
-  </si>
-  <si>
-    <t>[435, 426, 439, 445, 430, 434, 431]</t>
-  </si>
-  <si>
-    <t>[436, 452, 442, 435, 426, 424, 444]</t>
-  </si>
-  <si>
-    <t>[410, 448, 442, 441, 450, 449]</t>
-  </si>
-  <si>
-    <t>[451, 453, 410, 447, 437, 425, 449, 435]</t>
-  </si>
-  <si>
-    <t>[447, 448, 450, 435, 433, 434, 432]</t>
-  </si>
-  <si>
-    <t>[447, 441, 449, 439, 430, 432]</t>
+    <t>[431, 432, 434, 449]</t>
+  </si>
+  <si>
+    <t>[444, 435, 433, 431, 449]</t>
+  </si>
+  <si>
+    <t>[448, 437, 444, 436, 449, 434, 445]</t>
+  </si>
+  <si>
+    <t>[437, 425, 438, 452, 435, 445]</t>
+  </si>
+  <si>
+    <t>[448, 425, 435, 436]</t>
+  </si>
+  <si>
+    <t>[429, 422, 453, 425, 452, 436]</t>
+  </si>
+  <si>
+    <t>[450, 444, 430, 426, 441, 443]</t>
+  </si>
+  <si>
+    <t>[424, 442, 443, 441]</t>
+  </si>
+  <si>
+    <t>[450, 447, 439, 440, 442, 443]</t>
+  </si>
+  <si>
+    <t>[408, 410, 447, 452, 445, 440, 424, 441]</t>
+  </si>
+  <si>
+    <t>[439, 428, 426, 440, 424, 441, 427]</t>
+  </si>
+  <si>
+    <t>[439, 430, 426, 434, 435, 431, 445]</t>
+  </si>
+  <si>
+    <t>[444, 452, 436, 435, 426, 442, 424]</t>
+  </si>
+  <si>
+    <t>[410, 448, 450, 449, 442, 441]</t>
+  </si>
+  <si>
+    <t>[451, 453, 410, 425, 447, 449, 435, 437]</t>
+  </si>
+  <si>
+    <t>[448, 450, 447, 435, 433, 432, 434]</t>
+  </si>
+  <si>
+    <t>[430, 439, 441, 432, 449, 447]</t>
   </si>
   <si>
     <t>[463, 410, 453, 418, 416, 448]</t>
   </si>
   <si>
-    <t>[429, 438, 436, 412, 445, 442, 411, 408]</t>
-  </si>
-  <si>
-    <t>[451, 418, 423, 422, 438, 448, 425]</t>
-  </si>
-  <si>
-    <t>[287, 456, 455, 392, 305, 295]</t>
-  </si>
-  <si>
-    <t>[454, 287, 286, 294, 296, 295, 297]</t>
-  </si>
-  <si>
-    <t>[454, 287, 356, 392, 394]</t>
-  </si>
-  <si>
-    <t>[416, 421, 463, 420, 389, 458, 423, 362, 459]</t>
-  </si>
-  <si>
-    <t>[391, 353, 389, 362, 457, 390]</t>
-  </si>
-  <si>
-    <t>[222, 463, 460, 389, 457, 461]</t>
-  </si>
-  <si>
-    <t>[222, 224, 255, 214, 218, 459, 461]</t>
-  </si>
-  <si>
-    <t>[460, 214, 389, 390, 459]</t>
+    <t>[408, 429, 411, 412, 438, 442, 436, 445]</t>
+  </si>
+  <si>
+    <t>[451, 422, 418, 423, 448, 438, 425]</t>
+  </si>
+  <si>
+    <t>[287, 392, 456, 455, 305, 295]</t>
+  </si>
+  <si>
+    <t>[287, 454, 294, 286, 297, 295, 296]</t>
+  </si>
+  <si>
+    <t>[356, 287, 392, 394, 454]</t>
+  </si>
+  <si>
+    <t>[416, 421, 463, 420, 423, 458, 389, 459, 362]</t>
+  </si>
+  <si>
+    <t>[457, 390, 389, 391, 362, 353]</t>
+  </si>
+  <si>
+    <t>[463, 222, 457, 461, 460, 389]</t>
+  </si>
+  <si>
+    <t>[222, 461, 224, 218, 459, 255, 214]</t>
+  </si>
+  <si>
+    <t>[214, 390, 460, 389, 459]</t>
   </si>
   <si>
     <t>[217, 221, 463, 250]</t>
   </si>
   <si>
-    <t>[462, 217, 451, 416, 222, 457, 459]</t>
-  </si>
-  <si>
-    <t>[70, 96, 410, 80, 405, 404, 406]</t>
-  </si>
-  <si>
-    <t>[166, 205, 144, 5, 141, 143]</t>
-  </si>
-  <si>
-    <t>[61, 220, 251, 247, 253]</t>
-  </si>
-  <si>
-    <t>[34, 205, 81, 78, 79]</t>
+    <t>[462, 451, 416, 217, 457, 222, 459]</t>
+  </si>
+  <si>
+    <t>[70, 96, 410, 80, 406, 404, 405]</t>
+  </si>
+  <si>
+    <t>[144, 141, 5, 166, 205, 143]</t>
+  </si>
+  <si>
+    <t>[61, 252, 220, 247, 251, 253]</t>
+  </si>
+  <si>
+    <t>[325, 327, 288, 289, 357]</t>
+  </si>
+  <si>
+    <t>Sweetwater</t>
   </si>
   <si>
     <t>Mykawa</t>
-  </si>
-  <si>
-    <t>Sweetwater</t>
   </si>
   <si>
     <t>Stafford</t>
@@ -1874,7 +1874,7 @@
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1894,7 +1894,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1914,7 +1914,7 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1934,7 +1934,7 @@
         <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1954,7 +1954,7 @@
         <v>13</v>
       </c>
       <c r="F10" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1974,7 +1974,7 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1994,7 +1994,7 @@
         <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2014,7 +2014,7 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2034,7 +2034,7 @@
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2074,7 +2074,7 @@
         <v>19</v>
       </c>
       <c r="F16" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2094,7 +2094,7 @@
         <v>20</v>
       </c>
       <c r="F17" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2114,7 +2114,7 @@
         <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2134,7 +2134,7 @@
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2154,7 +2154,7 @@
         <v>23</v>
       </c>
       <c r="F20" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2174,7 +2174,7 @@
         <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2194,7 +2194,7 @@
         <v>25</v>
       </c>
       <c r="F22" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2214,7 +2214,7 @@
         <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2254,7 +2254,7 @@
         <v>28</v>
       </c>
       <c r="F25" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2274,7 +2274,7 @@
         <v>29</v>
       </c>
       <c r="F26" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2314,7 +2314,7 @@
         <v>31</v>
       </c>
       <c r="F28" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2714,7 +2714,7 @@
         <v>51</v>
       </c>
       <c r="F48" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2874,7 +2874,7 @@
         <v>59</v>
       </c>
       <c r="F56" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2954,7 +2954,7 @@
         <v>63</v>
       </c>
       <c r="F60" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2974,7 +2974,7 @@
         <v>64</v>
       </c>
       <c r="F61" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2994,7 +2994,7 @@
         <v>65</v>
       </c>
       <c r="F62" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -3034,7 +3034,7 @@
         <v>67</v>
       </c>
       <c r="F64" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -3054,7 +3054,7 @@
         <v>68</v>
       </c>
       <c r="F65" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -3094,7 +3094,7 @@
         <v>70</v>
       </c>
       <c r="F67" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -3114,7 +3114,7 @@
         <v>71</v>
       </c>
       <c r="F68" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -3134,7 +3134,7 @@
         <v>72</v>
       </c>
       <c r="F69" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -3274,7 +3274,7 @@
         <v>15</v>
       </c>
       <c r="F76" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -3314,7 +3314,7 @@
         <v>78</v>
       </c>
       <c r="F78" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -3334,7 +3334,7 @@
         <v>79</v>
       </c>
       <c r="F79" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -3434,7 +3434,7 @@
         <v>84</v>
       </c>
       <c r="F84" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3634,7 +3634,7 @@
         <v>94</v>
       </c>
       <c r="F94" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -4154,7 +4154,7 @@
         <v>118</v>
       </c>
       <c r="F120" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -4174,7 +4174,7 @@
         <v>119</v>
       </c>
       <c r="F121" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -4194,7 +4194,7 @@
         <v>120</v>
       </c>
       <c r="F122" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -4414,7 +4414,7 @@
         <v>131</v>
       </c>
       <c r="F133" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -4434,7 +4434,7 @@
         <v>132</v>
       </c>
       <c r="F134" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -4454,7 +4454,7 @@
         <v>133</v>
       </c>
       <c r="F135" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -4494,7 +4494,7 @@
         <v>19</v>
       </c>
       <c r="F137" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -4514,7 +4514,7 @@
         <v>134</v>
       </c>
       <c r="F138" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -4534,7 +4534,7 @@
         <v>135</v>
       </c>
       <c r="F139" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -4554,7 +4554,7 @@
         <v>136</v>
       </c>
       <c r="F140" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -4574,7 +4574,7 @@
         <v>137</v>
       </c>
       <c r="F141" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -4594,7 +4594,7 @@
         <v>138</v>
       </c>
       <c r="F142" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -4614,7 +4614,7 @@
         <v>139</v>
       </c>
       <c r="F143" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4634,7 +4634,7 @@
         <v>140</v>
       </c>
       <c r="F144" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4654,7 +4654,7 @@
         <v>141</v>
       </c>
       <c r="F145" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -4694,7 +4694,7 @@
         <v>143</v>
       </c>
       <c r="F147" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -4714,7 +4714,7 @@
         <v>144</v>
       </c>
       <c r="F148" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -4734,7 +4734,7 @@
         <v>145</v>
       </c>
       <c r="F149" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -4754,7 +4754,7 @@
         <v>146</v>
       </c>
       <c r="F150" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -4794,7 +4794,7 @@
         <v>148</v>
       </c>
       <c r="F152" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -4814,7 +4814,7 @@
         <v>149</v>
       </c>
       <c r="F153" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -4834,7 +4834,7 @@
         <v>150</v>
       </c>
       <c r="F154" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -4854,7 +4854,7 @@
         <v>151</v>
       </c>
       <c r="F155" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -4874,7 +4874,7 @@
         <v>152</v>
       </c>
       <c r="F156" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -4894,7 +4894,7 @@
         <v>153</v>
       </c>
       <c r="F157" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -4914,7 +4914,7 @@
         <v>154</v>
       </c>
       <c r="F158" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -4934,7 +4934,7 @@
         <v>155</v>
       </c>
       <c r="F159" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -5114,7 +5114,7 @@
         <v>164</v>
       </c>
       <c r="F168" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -5234,7 +5234,7 @@
         <v>170</v>
       </c>
       <c r="F174" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -5254,7 +5254,7 @@
         <v>171</v>
       </c>
       <c r="F175" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -5274,7 +5274,7 @@
         <v>172</v>
       </c>
       <c r="F176" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -5294,7 +5294,7 @@
         <v>173</v>
       </c>
       <c r="F177" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -5334,7 +5334,7 @@
         <v>175</v>
       </c>
       <c r="F179" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="180" spans="1:6">
@@ -5354,7 +5354,7 @@
         <v>176</v>
       </c>
       <c r="F180" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="181" spans="1:6">
@@ -5374,7 +5374,7 @@
         <v>177</v>
       </c>
       <c r="F181" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -5394,7 +5394,7 @@
         <v>178</v>
       </c>
       <c r="F182" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -5414,7 +5414,7 @@
         <v>179</v>
       </c>
       <c r="F183" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -5474,7 +5474,7 @@
         <v>182</v>
       </c>
       <c r="F186" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -5754,7 +5754,7 @@
         <v>196</v>
       </c>
       <c r="F200" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -5774,7 +5774,7 @@
         <v>197</v>
       </c>
       <c r="F201" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -5814,7 +5814,7 @@
         <v>199</v>
       </c>
       <c r="F203" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -5854,7 +5854,7 @@
         <v>201</v>
       </c>
       <c r="F205" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -6714,7 +6714,7 @@
         <v>208</v>
       </c>
       <c r="F248" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="249" spans="1:6">
@@ -7014,7 +7014,7 @@
         <v>257</v>
       </c>
       <c r="F263" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="264" spans="1:6">
@@ -7134,7 +7134,7 @@
         <v>263</v>
       </c>
       <c r="F269" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="270" spans="1:6">
@@ -7174,7 +7174,7 @@
         <v>265</v>
       </c>
       <c r="F271" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="272" spans="1:6">
@@ -7274,7 +7274,7 @@
         <v>270</v>
       </c>
       <c r="F276" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="277" spans="1:6">
@@ -7334,7 +7334,7 @@
         <v>273</v>
       </c>
       <c r="F279" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="280" spans="1:6">
@@ -7514,7 +7514,7 @@
         <v>282</v>
       </c>
       <c r="F288" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="289" spans="1:6">
@@ -7534,7 +7534,7 @@
         <v>283</v>
       </c>
       <c r="F289" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="290" spans="1:6">
@@ -7614,7 +7614,7 @@
         <v>287</v>
       </c>
       <c r="F293" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="294" spans="1:6">
@@ -7634,7 +7634,7 @@
         <v>288</v>
       </c>
       <c r="F294" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="295" spans="1:6">
@@ -7674,7 +7674,7 @@
         <v>290</v>
       </c>
       <c r="F296" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="297" spans="1:6">
@@ -7694,7 +7694,7 @@
         <v>291</v>
       </c>
       <c r="F297" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="298" spans="1:6">
@@ -7714,7 +7714,7 @@
         <v>292</v>
       </c>
       <c r="F298" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="299" spans="1:6">
@@ -7734,7 +7734,7 @@
         <v>293</v>
       </c>
       <c r="F299" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="300" spans="1:6">
@@ -7794,7 +7794,7 @@
         <v>296</v>
       </c>
       <c r="F302" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="303" spans="1:6">
@@ -7814,7 +7814,7 @@
         <v>297</v>
       </c>
       <c r="F303" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="304" spans="1:6">
@@ -7834,7 +7834,7 @@
         <v>298</v>
       </c>
       <c r="F304" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="305" spans="1:6">
@@ -7854,7 +7854,7 @@
         <v>299</v>
       </c>
       <c r="F305" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="306" spans="1:6">
@@ -7874,7 +7874,7 @@
         <v>300</v>
       </c>
       <c r="F306" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="307" spans="1:6">
@@ -7894,7 +7894,7 @@
         <v>301</v>
       </c>
       <c r="F307" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="308" spans="1:6">
@@ -7914,7 +7914,7 @@
         <v>302</v>
       </c>
       <c r="F308" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="309" spans="1:6">
@@ -7954,7 +7954,7 @@
         <v>304</v>
       </c>
       <c r="F310" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="311" spans="1:6">
@@ -7974,7 +7974,7 @@
         <v>305</v>
       </c>
       <c r="F311" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="312" spans="1:6">
@@ -7994,7 +7994,7 @@
         <v>306</v>
       </c>
       <c r="F312" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="313" spans="1:6">
@@ -8014,7 +8014,7 @@
         <v>307</v>
       </c>
       <c r="F313" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="314" spans="1:6">
@@ -8034,7 +8034,7 @@
         <v>308</v>
       </c>
       <c r="F314" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="315" spans="1:6">
@@ -8054,7 +8054,7 @@
         <v>309</v>
       </c>
       <c r="F315" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="316" spans="1:6">
@@ -8074,7 +8074,7 @@
         <v>310</v>
       </c>
       <c r="F316" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="317" spans="1:6">
@@ -8094,7 +8094,7 @@
         <v>311</v>
       </c>
       <c r="F317" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="318" spans="1:6">
@@ -8114,7 +8114,7 @@
         <v>312</v>
       </c>
       <c r="F318" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="319" spans="1:6">
@@ -8134,7 +8134,7 @@
         <v>313</v>
       </c>
       <c r="F319" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="320" spans="1:6">
@@ -8154,7 +8154,7 @@
         <v>314</v>
       </c>
       <c r="F320" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="321" spans="1:6">
@@ -8174,7 +8174,7 @@
         <v>315</v>
       </c>
       <c r="F321" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="322" spans="1:6">
@@ -8194,7 +8194,7 @@
         <v>316</v>
       </c>
       <c r="F322" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="323" spans="1:6">
@@ -8214,7 +8214,7 @@
         <v>317</v>
       </c>
       <c r="F323" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="324" spans="1:6">
@@ -8234,7 +8234,7 @@
         <v>318</v>
       </c>
       <c r="F324" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="325" spans="1:6">
@@ -8254,7 +8254,7 @@
         <v>319</v>
       </c>
       <c r="F325" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="326" spans="1:6">
@@ -8474,7 +8474,7 @@
         <v>328</v>
       </c>
       <c r="F336" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="337" spans="1:6">
@@ -8594,7 +8594,7 @@
         <v>334</v>
       </c>
       <c r="F342" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="343" spans="1:6">
@@ -8634,7 +8634,7 @@
         <v>336</v>
       </c>
       <c r="F344" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="345" spans="1:6">
@@ -8694,7 +8694,7 @@
         <v>339</v>
       </c>
       <c r="F347" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="348" spans="1:6">
@@ -8734,7 +8734,7 @@
         <v>341</v>
       </c>
       <c r="F349" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="350" spans="1:6">
@@ -8774,7 +8774,7 @@
         <v>343</v>
       </c>
       <c r="F351" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
     </row>
     <row r="352" spans="1:6">
@@ -8854,7 +8854,7 @@
         <v>347</v>
       </c>
       <c r="F355" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="356" spans="1:6">
@@ -8914,7 +8914,7 @@
         <v>350</v>
       </c>
       <c r="F358" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="359" spans="1:6">
@@ -9014,7 +9014,7 @@
         <v>355</v>
       </c>
       <c r="F363" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="364" spans="1:6">
@@ -9034,7 +9034,7 @@
         <v>356</v>
       </c>
       <c r="F364" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="365" spans="1:6">
@@ -9074,7 +9074,7 @@
         <v>358</v>
       </c>
       <c r="F366" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="367" spans="1:6">
@@ -9214,7 +9214,7 @@
         <v>363</v>
       </c>
       <c r="F373" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="374" spans="1:6">
@@ -9254,7 +9254,7 @@
         <v>365</v>
       </c>
       <c r="F375" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="376" spans="1:6">
@@ -9554,7 +9554,7 @@
         <v>380</v>
       </c>
       <c r="F390" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="391" spans="1:6">
@@ -9634,7 +9634,7 @@
         <v>384</v>
       </c>
       <c r="F394" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="395" spans="1:6">
@@ -9654,7 +9654,7 @@
         <v>385</v>
       </c>
       <c r="F395" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="396" spans="1:6">
@@ -9674,7 +9674,7 @@
         <v>386</v>
       </c>
       <c r="F396" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="397" spans="1:6">
@@ -9694,7 +9694,7 @@
         <v>387</v>
       </c>
       <c r="F397" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="398" spans="1:6">
@@ -9714,7 +9714,7 @@
         <v>388</v>
       </c>
       <c r="F398" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="399" spans="1:6">
@@ -9734,7 +9734,7 @@
         <v>389</v>
       </c>
       <c r="F399" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="400" spans="1:6">
@@ -9754,7 +9754,7 @@
         <v>390</v>
       </c>
       <c r="F400" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="401" spans="1:6">
@@ -9774,7 +9774,7 @@
         <v>391</v>
       </c>
       <c r="F401" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="402" spans="1:6">
@@ -9814,7 +9814,7 @@
         <v>392</v>
       </c>
       <c r="F403" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="404" spans="1:6">
@@ -9834,7 +9834,7 @@
         <v>393</v>
       </c>
       <c r="F404" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="405" spans="1:6">
@@ -9854,7 +9854,7 @@
         <v>394</v>
       </c>
       <c r="F405" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="406" spans="1:6">
@@ -9934,7 +9934,7 @@
         <v>398</v>
       </c>
       <c r="F409" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="410" spans="1:6">
@@ -10074,7 +10074,7 @@
         <v>405</v>
       </c>
       <c r="F416" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="417" spans="1:6">
@@ -10134,7 +10134,7 @@
         <v>408</v>
       </c>
       <c r="F419" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="420" spans="1:6">
@@ -10154,7 +10154,7 @@
         <v>409</v>
       </c>
       <c r="F420" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="421" spans="1:6">
@@ -10174,7 +10174,7 @@
         <v>410</v>
       </c>
       <c r="F421" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="422" spans="1:6">
@@ -10194,7 +10194,7 @@
         <v>411</v>
       </c>
       <c r="F422" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="423" spans="1:6">
@@ -10234,7 +10234,7 @@
         <v>413</v>
       </c>
       <c r="F424" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="425" spans="1:6">
@@ -10254,7 +10254,7 @@
         <v>414</v>
       </c>
       <c r="F425" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="426" spans="1:6">
@@ -10354,7 +10354,7 @@
         <v>418</v>
       </c>
       <c r="F430" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="431" spans="1:6">
@@ -10394,7 +10394,7 @@
         <v>420</v>
       </c>
       <c r="F432" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="433" spans="1:6">
@@ -10794,7 +10794,7 @@
         <v>439</v>
       </c>
       <c r="F452" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="453" spans="1:6">
@@ -10854,7 +10854,7 @@
         <v>442</v>
       </c>
       <c r="F455" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="456" spans="1:6">
@@ -10874,7 +10874,7 @@
         <v>443</v>
       </c>
       <c r="F456" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="457" spans="1:6">
@@ -10894,7 +10894,7 @@
         <v>444</v>
       </c>
       <c r="F457" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="458" spans="1:6">
@@ -10914,7 +10914,7 @@
         <v>445</v>
       </c>
       <c r="F458" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="459" spans="1:6">
@@ -11082,19 +11082,19 @@
         <v>465</v>
       </c>
       <c r="B467">
-        <v>-95.3211</v>
+        <v>-95.32125610590822</v>
       </c>
       <c r="C467">
-        <v>29.6759</v>
+        <v>29.67578534220857</v>
       </c>
       <c r="D467">
-        <v>326.25</v>
+        <v>290</v>
       </c>
       <c r="E467" t="s">
         <v>454</v>
       </c>
       <c r="F467" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="468" spans="1:6">
@@ -11102,13 +11102,13 @@
         <v>466</v>
       </c>
       <c r="B468">
-        <v>-95.5557</v>
+        <v>-95.55583702616946</v>
       </c>
       <c r="C468">
-        <v>29.6194</v>
+        <v>29.61935353306665</v>
       </c>
       <c r="D468">
-        <v>326.25</v>
+        <v>290</v>
       </c>
       <c r="E468" t="s">
         <v>455</v>
@@ -11122,19 +11122,19 @@
         <v>467</v>
       </c>
       <c r="B469">
-        <v>-95.2895</v>
+        <v>-95.40848234626999</v>
       </c>
       <c r="C469">
-        <v>29.6395</v>
+        <v>29.88062033368866</v>
       </c>
       <c r="D469">
-        <v>217.5</v>
+        <v>290</v>
       </c>
       <c r="E469" t="s">
         <v>456</v>
       </c>
       <c r="F469" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>